<commit_message>
timestamp added to file upload
</commit_message>
<xml_diff>
--- a/logs/Failed/Duplicate-Compounds.xlsx
+++ b/logs/Failed/Duplicate-Compounds.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,70 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2024-09-03 12:18:17</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>ORM-0515835</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Z195631098</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>C18H19CL2N5OS</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Duplicate</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2024-09-03 12:18:18</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ORM-0515836</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Z2754556176</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>C17H28N4O2</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Duplicate</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/examples/compound_test.sdf</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
normalize and map supplier names to materials_table.json
</commit_message>
<xml_diff>
--- a/logs/Failed/Duplicate-Compounds.xlsx
+++ b/logs/Failed/Duplicate-Compounds.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,6 +593,70 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2024-10-28 18:36:25</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>ORM-0516041</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>MCULE-2227031507</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>C21H17CLN2O2</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Duplicate</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/MCULE/mcule_test.sdf</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2024-10-28 18:36:27</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>ORM-0516042</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>MCULE-3988458386</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>C16H14CLN5O</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Duplicate</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>/home/robekott/ERAT/MCULE/mcule_test.sdf</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>